<commit_message>
Revised Sample Size, Tables, Results
</commit_message>
<xml_diff>
--- a/Table 4.xlsx
+++ b/Table 4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\PhD-Study-IV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E472F5-B808-482A-B513-BE3FF6D8DE4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665532AB-1202-4002-9E88-74F602CC7796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0AA141E9-734F-49F6-AF46-17E5186CD78A}"/>
   </bookViews>
@@ -171,12 +171,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -184,6 +178,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,7 +501,7 @@
   <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,447 +513,452 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5" t="s">
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5" t="s">
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5" t="s">
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5" t="s">
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5" t="s">
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
+      <c r="A2" s="12"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="11"/>
       <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="G2" s="11"/>
       <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="5"/>
+      <c r="J2" s="11"/>
       <c r="K2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="5"/>
+      <c r="M2" s="11"/>
       <c r="N2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="5"/>
+      <c r="P2" s="11"/>
       <c r="Q2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="S2" s="5"/>
+      <c r="S2" s="11"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="7">
-        <v>1</v>
-      </c>
-      <c r="F3" s="7">
-        <v>1</v>
-      </c>
-      <c r="G3" s="7">
-        <v>1</v>
-      </c>
-      <c r="H3" s="7">
-        <v>1</v>
-      </c>
-      <c r="I3" s="7">
-        <v>1</v>
-      </c>
-      <c r="J3" s="7">
-        <v>1</v>
-      </c>
-      <c r="K3" s="7">
-        <v>1</v>
-      </c>
-      <c r="L3" s="7">
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5">
+        <v>1</v>
+      </c>
+      <c r="I3" s="5">
+        <v>1</v>
+      </c>
+      <c r="J3" s="5">
+        <v>1</v>
+      </c>
+      <c r="K3" s="5">
+        <v>1</v>
+      </c>
+      <c r="L3" s="5">
         <v>0.37</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="5">
         <v>1.3</v>
       </c>
-      <c r="N3" s="7">
-        <v>1</v>
-      </c>
-      <c r="O3" s="7">
-        <v>1</v>
-      </c>
-      <c r="P3" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="7">
-        <v>1</v>
-      </c>
-      <c r="R3" s="7">
-        <v>1</v>
-      </c>
-      <c r="S3" s="7">
-        <v>1</v>
-      </c>
-      <c r="T3" s="8"/>
+      <c r="N3" s="5">
+        <v>1</v>
+      </c>
+      <c r="O3" s="5">
+        <v>1</v>
+      </c>
+      <c r="P3" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>1</v>
+      </c>
+      <c r="R3" s="5">
+        <v>1</v>
+      </c>
+      <c r="S3" s="5">
+        <v>1</v>
+      </c>
+      <c r="T3" s="6"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="7">
         <v>-4.5599999999999996</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="8">
         <v>-8.43</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="8">
         <v>-0.7</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="5">
         <v>0.77</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="5">
         <v>0.51</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="5">
         <v>1.1499999999999999</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="5">
         <v>0.82</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="5">
         <v>0.54</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="5">
         <v>1.24</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="9">
         <v>0.7</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="5">
         <v>0.47</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="9">
         <v>1.05</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="9">
         <v>0.54</v>
       </c>
-      <c r="O4" s="11">
+      <c r="O4" s="9">
         <v>0.27</v>
       </c>
-      <c r="P4" s="7">
+      <c r="P4" s="5">
         <v>1.04</v>
       </c>
-      <c r="Q4" s="7">
+      <c r="Q4" s="3">
         <v>1.31</v>
       </c>
-      <c r="R4" s="7">
+      <c r="R4" s="5">
         <v>0.86</v>
       </c>
-      <c r="S4" s="7">
+      <c r="S4" s="5">
         <v>1.97</v>
       </c>
-      <c r="T4" s="8"/>
+      <c r="T4" s="6"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="8">
         <v>-2.38</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="8">
         <v>-8.9600000000000009</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="8">
         <v>4.12</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="5">
         <v>0.72</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="5">
         <v>0.36</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="5">
         <v>1.41</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="5">
         <v>0.66</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="5">
         <v>0.33</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="5">
         <v>1.31</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="5">
         <v>0.73</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="5">
         <v>0.37</v>
       </c>
-      <c r="M5" s="11">
+      <c r="M5" s="9">
         <v>1.44</v>
       </c>
-      <c r="N5" s="11">
+      <c r="N5" s="9">
         <v>0.31</v>
       </c>
-      <c r="O5" s="11">
+      <c r="O5" s="9">
         <v>0.35</v>
       </c>
-      <c r="P5" s="7">
+      <c r="P5" s="5">
         <v>0.82</v>
       </c>
-      <c r="Q5" s="12">
+      <c r="Q5" s="10">
         <v>1.35</v>
       </c>
-      <c r="R5" s="7">
+      <c r="R5" s="5">
         <v>0.68</v>
       </c>
-      <c r="S5" s="7">
+      <c r="S5" s="5">
         <v>2.67</v>
       </c>
-      <c r="T5" s="8"/>
+      <c r="T5" s="6"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="8">
         <v>0.63</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="8">
         <v>-5.41</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="8">
         <v>6.67</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <v>0.78</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="5">
         <v>0.41</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="5">
         <v>1.47</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="5">
         <v>0.74</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="5">
         <v>0.39</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="5">
         <v>1.42</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="5">
         <v>0.7</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="5">
         <v>0.7606832</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6" s="9">
         <v>2.3066355999999999</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6" s="9">
         <v>0.54</v>
       </c>
-      <c r="O6" s="11">
+      <c r="O6" s="9">
         <v>0.13</v>
       </c>
-      <c r="P6" s="7">
+      <c r="P6" s="5">
         <v>0.7</v>
       </c>
       <c r="Q6" s="3">
         <v>1.59</v>
       </c>
-      <c r="R6" s="7">
+      <c r="R6" s="5">
         <v>0.84</v>
       </c>
-      <c r="S6" s="7">
+      <c r="S6" s="5">
         <v>2.99</v>
       </c>
-      <c r="T6" s="8"/>
+      <c r="T6" s="6"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="8">
         <v>2.27</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="8">
         <v>-5.96</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="8">
         <v>10.51</v>
       </c>
       <c r="E7" s="3">
         <v>1.44</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="5">
         <v>0.61</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="5">
         <v>3.39</v>
       </c>
       <c r="H7" s="3">
         <v>1.1499999999999999</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="5">
         <v>0.49</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="5">
         <v>0.48</v>
       </c>
       <c r="K7" s="3">
         <v>1.4</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="5">
         <v>0.62</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="5">
         <v>3.4</v>
       </c>
       <c r="N7" s="3">
         <v>1.36</v>
       </c>
-      <c r="O7" s="7">
+      <c r="O7" s="5">
         <v>0.53</v>
       </c>
-      <c r="P7" s="7">
+      <c r="P7" s="5">
         <v>3.47</v>
       </c>
-      <c r="Q7" s="7">
+      <c r="Q7" s="5">
         <v>0.55000000000000004</v>
       </c>
-      <c r="R7" s="7">
+      <c r="R7" s="5">
         <v>0.23</v>
       </c>
-      <c r="S7" s="7">
+      <c r="S7" s="5">
         <v>1.31</v>
       </c>
-      <c r="T7" s="8"/>
+      <c r="T7" s="6"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="8">
         <v>-0.88</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="8">
         <v>-12.27</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="8">
         <v>10.5</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="5">
         <v>0.77</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="5">
         <v>0.23</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="5">
         <v>2.57</v>
       </c>
       <c r="H8" s="3">
         <v>1.05</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="5">
         <v>0.34</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="5">
         <v>4.1399999999999997</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="5">
         <v>0.9</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="5">
         <v>0.26</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="5">
         <v>3.09</v>
       </c>
       <c r="N8" s="3">
         <v>3.43</v>
       </c>
-      <c r="O8" s="7">
+      <c r="O8" s="5">
         <v>0.91</v>
       </c>
-      <c r="P8" s="7">
+      <c r="P8" s="5">
         <v>12.8</v>
       </c>
-      <c r="Q8" s="7">
+      <c r="Q8" s="5">
         <v>0.77</v>
       </c>
-      <c r="R8" s="7">
+      <c r="R8" s="5">
         <v>0.23</v>
       </c>
-      <c r="S8" s="7">
+      <c r="S8" s="5">
         <v>2.5299999999999998</v>
       </c>
-      <c r="T8" s="8"/>
+      <c r="T8" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="O2:P2"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="B1:D1"/>
@@ -962,11 +967,6 @@
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="I2:J2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="O2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>